<commit_message>
chore: update 128 sem4 tt
</commit_message>
<xml_diff>
--- a/raw/time_tables/B.Tech 128 (btech-128)/4/1.xlsx
+++ b/raw/time_tables/B.Tech 128 (btech-128)/4/1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="464">
   <si>
     <t>B.TECH. II Yr( IV SEMESTER) TIMETABLE EVEN SEMESTER 2026, JIIT-128</t>
   </si>
@@ -82,52 +82,52 @@
     <t>PF7F8(XXXXXXX) -CL4/KHM/BHB</t>
   </si>
   <si>
+    <t>LALL(15B1NHS433) -153/SAV</t>
+  </si>
+  <si>
+    <t>LF16F17(24B11CS222) -138/GAH</t>
+  </si>
+  <si>
+    <t>PF1F2F3F4F5F6F7F9F10F11(25B16CS212)-151/RHN/HMV</t>
+  </si>
+  <si>
+    <t>LF16F17(24B11CS225) -118/DVG</t>
+  </si>
+  <si>
+    <t>LF16F17(24B11CS221) -118/MHS</t>
+  </si>
+  <si>
+    <t>LF1F2(24B11CS222) -111/MGO</t>
+  </si>
+  <si>
+    <t>LALL(16B1NHS332)-117/ALOK</t>
+  </si>
+  <si>
+    <t>TF1F2F7F8F9F10F11(15B1NHS433) -225
+/SAV</t>
+  </si>
+  <si>
+    <t>PF1F2F3F4(25B16CS211)-035//MSH/JSH/AKB</t>
+  </si>
+  <si>
+    <t>LF4F5F6(25B12CS211) -118/AKS</t>
+  </si>
+  <si>
+    <t>LF12F13F14F16F18F19E1E2E3E4
+(19B12HS412)-228/AMA</t>
+  </si>
+  <si>
+    <t>TF1F2F7F8F9F10F11(15B1NHS431) -229
+/EKS</t>
+  </si>
+  <si>
+    <t>LE3E4(24B41EC211) -138/ANG</t>
+  </si>
+  <si>
     <t>LF16F17F18(19B13BT211) -153
 /GUNJAN</t>
   </si>
   <si>
-    <t>LALL(15B1NHS433) -153/SAV</t>
-  </si>
-  <si>
-    <t>LF16F17(24B11CS222) -138/GAH</t>
-  </si>
-  <si>
-    <t>PF1F2F3F4F5F6F7F9F10F11(25B16CS212)-151/RHN/HMV</t>
-  </si>
-  <si>
-    <t>LF16F17(24B11CS225) -118/DVG</t>
-  </si>
-  <si>
-    <t>LF16F17(24B11CS221) -118/MHS</t>
-  </si>
-  <si>
-    <t>LF1F2(24B11CS222) -111/MGO</t>
-  </si>
-  <si>
-    <t>LALL(16B1NHS332)-117/ALOK</t>
-  </si>
-  <si>
-    <t>TF1F2F7F8F9F10F11(15B1NHS433) -225
-/SAV</t>
-  </si>
-  <si>
-    <t>PF1F2F3F4(25B16CS211)-035//MSH/JSH/AKB</t>
-  </si>
-  <si>
-    <t>LF4F5F6(25B12CS211) -118/AKS</t>
-  </si>
-  <si>
-    <t>LF12F13F14F16F18F19E1E2E3E4
-(19B12HS412)-228/AMA</t>
-  </si>
-  <si>
-    <t>TF1F2F7F8F9F10F11(15B1NHS431) -229
-/EKS</t>
-  </si>
-  <si>
-    <t>LE3E4(24B41EC211) -138/ANG</t>
-  </si>
-  <si>
     <t>PE4(18B15EC214) -256/MEA/SAK/MAK</t>
   </si>
   <si>
@@ -174,10 +174,7 @@
 /HIMANSHI</t>
   </si>
   <si>
-    <t>TE2(15B11EC411) --234/BHC</t>
-  </si>
-  <si>
-    <t>TE1(24B41EC211) -225/ANK</t>
+    <t>TE1(24B41EC211) -113/ANK</t>
   </si>
   <si>
     <t>TF18(24B11CS221) -244/BAIBHAV</t>
@@ -193,6 +190,12 @@
     <t>TF11(24B11CS221) -229/BAIBHAV</t>
   </si>
   <si>
+    <t>TE3(24B41EC211) -244B/ANK</t>
+  </si>
+  <si>
+    <t>LF18F19(24B11CS223) -153/KHM</t>
+  </si>
+  <si>
     <t>TUES</t>
   </si>
   <si>
@@ -215,7 +218,7 @@
     <t>PF11(25B15EC311) -257/AJK/RKV</t>
   </si>
   <si>
-    <t>PF6(25B15EC311) -257/RUS/MEA/MAK</t>
+    <t>PF6(25B15EC311) -257/KDT/MEA/MAK</t>
   </si>
   <si>
     <t>PF4F5F6(24B15CS221) - CL2/MIT/NRP/ANU/NAVED</t>
@@ -298,6 +301,9 @@
 PF7(25B15EC311) -257/VKM/RAS</t>
   </si>
   <si>
+    <t>TE2(15B11EC411) --234/BHC</t>
+  </si>
+  <si>
     <t>LF3F4(XXXXXXX) -111/KHM</t>
   </si>
   <si>
@@ -360,7 +366,7 @@
     <t>LE3E4(24B41EC211) -CR54/ANG</t>
   </si>
   <si>
-    <t>LALL(25B42EC212) -244B/VKT</t>
+    <t>LALL(25B42EC212) -244B/VIT</t>
   </si>
   <si>
     <t>LF1F2F3(19B13BT211) -SR05/MANISHA</t>
@@ -454,7 +460,7 @@
     <t>LE3E4(15B11EC411) -CR54/ATK</t>
   </si>
   <si>
-    <t>LF18F19(24B11CS223) -123/KHM</t>
+    <t>LF16F17F18(19B13BT211) -117/GUNJAN</t>
   </si>
   <si>
     <t>LF16F17(24B11CS225) -117/DVG</t>
@@ -524,9 +530,6 @@
     <t>TF16(24B11CS221) -111/SHIVANI</t>
   </si>
   <si>
-    <t>LE3E4(18B11EC214) -226/MEA</t>
-  </si>
-  <si>
     <t>PF14F16F17F18 F19(25B16CS211)-035/AKB/JSH/ADS/MSH</t>
   </si>
   <si>
@@ -616,7 +619,7 @@
     <t>LE1E2(24B41EC211) -244B/ANG</t>
   </si>
   <si>
-    <t>PF1(25B15EC311) -257/DKA/AJK</t>
+    <t>PF1(25B15EC311) -257/DIVYA/AJK</t>
   </si>
   <si>
     <t>TF12(24B11CS221) -127/JATIN</t>
@@ -638,6 +641,9 @@
   </si>
   <si>
     <t>TF3F4F5F6F13(15B1NHS433) -225/SAV</t>
+  </si>
+  <si>
+    <t>TE4(18B11EC214) -244/MEA</t>
   </si>
   <si>
     <t>TF17(24B11CS225) -3044/TWINKLE</t>
@@ -712,7 +718,7 @@
     <t>TE1E2E3E4(19B12HS412)-116/AMA</t>
   </si>
   <si>
-    <t>PF2(25B15EC311) -257/DKA/KDT</t>
+    <t>PF2(25B15EC311) -257/DIVYA/KDT</t>
   </si>
   <si>
     <t>LF11F12(24B11CS223) -123/SHR</t>
@@ -757,7 +763,7 @@
     <t>TF1(24B11CS221) -116/JATIN</t>
   </si>
   <si>
-    <t>LF3F4(24B11CS222) -153/SGU</t>
+    <t>LF3F4(25B11EC311) -153/DIVYA</t>
   </si>
   <si>
     <t>TF7F8F3(19B12HS412)-116/AMA</t>
@@ -810,10 +816,7 @@
     <t>TE2(24B41EC211) -244B/ANK</t>
   </si>
   <si>
-    <t>TE4(18B11EC214) -244/MEA</t>
-  </si>
-  <si>
-    <t>TE3(24B41EC211) -244B/ANK</t>
+    <t>LE3E4(18B11EC214) -111/MEA</t>
   </si>
   <si>
     <t>SAT</t>
@@ -832,6 +835,9 @@
   </si>
   <si>
     <t>PF13F14F16(24B15CS222) -151/RKA/SHR/AYP/ZUBAIR</t>
+  </si>
+  <si>
+    <t>LE3E4(18B11EC214) -3084/MEA</t>
   </si>
   <si>
     <t>PF11F12(XXXXXXX) -CL4/HMA/ANK/BHB</t>
@@ -877,10 +883,10 @@
     <t>LF5F6(24B11CS221) -CR54/TWT</t>
   </si>
   <si>
+    <t>LE1E2(15B11EC411) -111/BHC</t>
+  </si>
+  <si>
     <t>LF1F2(25B11EC311) -118/DIVYA</t>
-  </si>
-  <si>
-    <t>LF3F4(25B11EC311) -CR53/DIVYA</t>
   </si>
   <si>
     <t>LF13F14(25B11EC311) -138/PRK</t>
@@ -1116,7 +1122,7 @@
     <t>Divya Kaushik</t>
   </si>
   <si>
-    <t>DKA/DIVYA</t>
+    <t>DIVYA/DIVYA</t>
   </si>
   <si>
     <t>Atul Kumar</t>
@@ -1696,15 +1702,15 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="42.86"/>
-    <col customWidth="1" min="2" max="2" width="36.71"/>
-    <col customWidth="1" min="3" max="3" width="32.86"/>
-    <col customWidth="1" min="4" max="4" width="55.43"/>
-    <col customWidth="1" min="5" max="5" width="49.86"/>
-    <col customWidth="1" min="6" max="6" width="53.29"/>
-    <col customWidth="1" min="7" max="7" width="82.43"/>
-    <col customWidth="1" min="8" max="8" width="62.71"/>
-    <col customWidth="1" min="9" max="9" width="70.0"/>
+    <col customWidth="1" min="1" max="1" width="58.57"/>
+    <col customWidth="1" min="2" max="2" width="55.43"/>
+    <col customWidth="1" min="3" max="3" width="63.29"/>
+    <col customWidth="1" min="4" max="4" width="58.43"/>
+    <col customWidth="1" min="5" max="5" width="79.0"/>
+    <col customWidth="1" min="6" max="6" width="79.43"/>
+    <col customWidth="1" min="7" max="7" width="99.14"/>
+    <col customWidth="1" min="8" max="8" width="82.71"/>
+    <col customWidth="1" min="9" max="9" width="71.57"/>
     <col customWidth="1" min="10" max="26" width="8.71"/>
   </cols>
   <sheetData>
@@ -1785,37 +1791,34 @@
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8">
@@ -1826,19 +1829,19 @@
         <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9">
@@ -1855,7 +1858,7 @@
         <v>39</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>40</v>
@@ -1891,1720 +1894,1725 @@
       <c r="G11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="12">
       <c r="B12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>55</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="H17" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="B22" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="B23" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="C24" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="C25" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="C26" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="D27" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="D30" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="B31" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="D32" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="B33" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="B34" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="B35" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="B36" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="B37" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="B38" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1">
       <c r="D41" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="B44" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="B45" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="B46" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="B47" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="B48" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="B49" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="B50" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="B51" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="B52" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="B53" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="D54" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="H55" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="H56" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="H57" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="B59" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D59" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G59" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="H59" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="B60" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="B61" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="B62" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="B63" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="B64" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="B65" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="B66" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="B67" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="B68" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="69" ht="15.75" customHeight="1">
-      <c r="D69" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="69" ht="15.75" customHeight="1"/>
     <row r="70" ht="15.75" customHeight="1">
       <c r="D70" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="B73" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="B74" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="B75" s="1" t="s">
-        <v>17</v>
+        <v>264</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="B76" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="B77" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="B78" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="B79" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="B80" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1">
+      <c r="C83" s="1" t="s">
+        <v>279</v>
+      </c>
       <c r="D83" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="B84" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="D85" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="D86" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1"/>
     <row r="88" ht="15.75" customHeight="1">
       <c r="B88" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="B89" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="B90" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="B91" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="B92" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="B93" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="B94" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="B95" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="B96" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="B97" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="B98" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="B99" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="B100" s="1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="B101" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="B102" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="B103" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="B104" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="B105" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="B106" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="B107" s="1" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="B108" s="1" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="B109" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="B110" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="B111" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="B112" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="B113" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="B114" s="1" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="B115" s="1" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="B116" s="1" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="B117" s="1" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="B118" s="1" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="B119" s="1" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1"/>
     <row r="121" ht="15.75" customHeight="1"/>
     <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="1" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="1" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="1" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="1" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
chore: update 128 btech sem4
</commit_message>
<xml_diff>
--- a/raw/time_tables/B.Tech 128 (btech-128)/4/1.xlsx
+++ b/raw/time_tables/B.Tech 128 (btech-128)/4/1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Timetable" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Timetable" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="465">
   <si>
     <t>B.TECH. II Yr( IV SEMESTER) TIMETABLE EVEN SEMESTER 2026, JIIT-128</t>
   </si>
@@ -44,7 +44,7 @@
     <t>MON</t>
   </si>
   <si>
-    <t>PF1F2F3(24B15CS221) - CL2/KSA/NRP/ANU/VAIBHAV</t>
+    <t>PF1F2F3(24B15CS221) - CL2/NRP/ANU/JATIN</t>
   </si>
   <si>
     <t>LE1E2(18B11EC214) -226/SVS</t>
@@ -63,7 +63,7 @@
     <t>PE1(24B45EC211) -256/HIG/PRK</t>
   </si>
   <si>
-    <t>PF4F5F6(24B15CS222) -151/RKA/SHR/AKS/FARAZ</t>
+    <t>PF4F5F6(24B15CS222) -151/RKA/SHR/AMS/ZUBAIR</t>
   </si>
   <si>
     <t>LE3E4(18B11EC214) -228/MEA</t>
@@ -79,7 +79,7 @@
     <t>PF8(25B15EC311) -257/AJK/ATK/DKS</t>
   </si>
   <si>
-    <t>PF7F8(XXXXXXX) -CL4/KHM/BHB</t>
+    <t>PF7F8(XXXXXXX) -CL4/KHM/ANK</t>
   </si>
   <si>
     <t>LALL(15B1NHS433) -153/SAV</t>
@@ -88,13 +88,13 @@
     <t>LF16F17(24B11CS222) -138/GAH</t>
   </si>
   <si>
-    <t>PF1F2F3F4F5F6F7F9F10F11(25B16CS212)-151/RHN/HMV</t>
+    <t>PF1F2F3F4F5F6F7F9F10F11(25B16CS212)-151/RHN/HMV/KESHAN</t>
   </si>
   <si>
     <t>LF16F17(24B11CS225) -118/DVG</t>
   </si>
   <si>
-    <t>LF16F17(24B11CS221) -118/MHS</t>
+    <t>LF16F17(24B11CS221) -118/DTS</t>
   </si>
   <si>
     <t>LF1F2(24B11CS222) -111/MGO</t>
@@ -107,7 +107,7 @@
 /SAV</t>
   </si>
   <si>
-    <t>PF1F2F3F4(25B16CS211)-035//MSH/JSH/AKB</t>
+    <t>PF1F2F3F4F9(25B16CS211)-035//MSH/JSH/AKB</t>
   </si>
   <si>
     <t>LF4F5F6(25B12CS211) -118/AKS</t>
@@ -117,15 +117,11 @@
 (19B12HS412)-228/AMA</t>
   </si>
   <si>
-    <t>TF1F2F7F8F9F10F11(15B1NHS431) -229
-/EKS</t>
+    <t>TF1F2F7F8F9F10F11F12F18(15B1NHS431) 
+-229/EKS</t>
   </si>
   <si>
     <t>LE3E4(24B41EC211) -138/ANG</t>
-  </si>
-  <si>
-    <t>LF16F17F18(19B13BT211) -153
-/GUNJAN</t>
   </si>
   <si>
     <t>PE4(18B15EC214) -256/MEA/SAK/MAK</t>
@@ -141,10 +137,17 @@
 /PRS</t>
   </si>
   <si>
+    <t>TF18(24B11CS225) -127/TWINKLE 
+HANDA</t>
+  </si>
+  <si>
     <t>LF13F14(24B11CS223) -230/VKG</t>
   </si>
   <si>
     <t>PF9(25B15EC311) -257/PAA/HIG</t>
+  </si>
+  <si>
+    <t>LF18F19(24B11CS223) -153/KHM</t>
   </si>
   <si>
     <t>LALL(15B1NHS433)-SR05/AKS</t>
@@ -154,16 +157,10 @@
 /ALOK</t>
   </si>
   <si>
-    <t>LF13F14(XXXXXXX) -230/KHM</t>
-  </si>
-  <si>
     <t>TE2(18B11EC214) -127/SVS</t>
   </si>
   <si>
-    <t>LF11F12(25B11EC311) -138/PAA</t>
-  </si>
-  <si>
-    <t>TF19(24B11CS225) -126/TWINKLE</t>
+    <t>LF11F12(XXXXXXX) -138/BHB</t>
   </si>
   <si>
     <t>TF1F2F4F9F10F11(19B12HS412)-225/HSS 
@@ -180,7 +177,7 @@
     <t>TF18(24B11CS221) -244/BAIBHAV</t>
   </si>
   <si>
-    <t>LF11F12(XXXXXXX) -138/BHB</t>
+    <t>LF11F12(25B11EC311) -138/PAA</t>
   </si>
   <si>
     <t>TF1F2F7F8F9F10F11(15B1NHS433)-244
@@ -193,9 +190,6 @@
     <t>TE3(24B41EC211) -244B/ANK</t>
   </si>
   <si>
-    <t>LF18F19(24B11CS223) -153/KHM</t>
-  </si>
-  <si>
     <t>TUES</t>
   </si>
   <si>
@@ -205,11 +199,7 @@
     <t>LF16F17(24B11CS222) -111/GAH</t>
   </si>
   <si>
-    <t>LF10F11F12(19B13BT211) -SR05/NIVEDITA</t>
-  </si>
-  <si>
-    <t>LF10F11F12(19B13BT211) -
-SR05/NIVEDITA</t>
+    <t>LF10F11F12(19B13BT211) -254/NIVEDITA</t>
   </si>
   <si>
     <t>PF9F10(XXXXXXX) -CL4/BHB/HMA</t>
@@ -218,10 +208,10 @@
     <t>PF11(25B15EC311) -257/AJK/RKV</t>
   </si>
   <si>
-    <t>PF6(25B15EC311) -257/KDT/MEA/MAK</t>
-  </si>
-  <si>
-    <t>PF4F5F6(24B15CS221) - CL2/MIT/NRP/ANU/NAVED</t>
+    <t>PF6(25B15EC311) -257/KDT/MEA</t>
+  </si>
+  <si>
+    <t>PF4F5F6(24B15CS221) - CL2/MIT/NRP/VAIBHAV</t>
   </si>
   <si>
     <t>LF13F14F17(25B12CS211) -117/MSH</t>
@@ -236,22 +226,22 @@
     <t>LF7F8F9(25B12CS211) -148/AKB</t>
   </si>
   <si>
-    <t>PF1F2F3(24B15CS222) -151//MGO/AMS/FARAZ</t>
+    <t>PF1F2F3(24B15CS222) -151//MGO/AKS/FARAZ</t>
   </si>
   <si>
     <t>LF16F18F19(25B12CS211) -118/KISHAN</t>
   </si>
   <si>
-    <t>PF8F12F13F14F16F17F18F19(25B16CS212)-151//RHN/HMV</t>
-  </si>
-  <si>
-    <t>LF7F8(XXXXXXX) -148/MHS</t>
+    <t>PF8F12F13F14F16F17F18F19(25B16CS212)-151//RHN/HMV/KESHAN</t>
+  </si>
+  <si>
+    <t>LF7F8(XXXXXXX) -148/BHB</t>
   </si>
   <si>
     <t>LF1F2(24B11CS221) -117/NRP</t>
   </si>
   <si>
-    <t>PF13F14(XXXXXXX) -CL1/MHS/JYR/KHM</t>
+    <t>PF13F14(XXXXXXX) -CL1/NISHANT/JYR/KHM</t>
   </si>
   <si>
     <t>LF3F4(24B11CS222) -111/SGU</t>
@@ -263,10 +253,10 @@
     <t>LF13F14(24B11CS222) -153/RKA</t>
   </si>
   <si>
-    <t>LF3F4(24B11CS221) -111/KSA</t>
-  </si>
-  <si>
-    <t>PF18F19(24B15CS215) -AI LAB//PRM/SHIVANI</t>
+    <t>LF3F4(24B11CS221) -138/KSA</t>
+  </si>
+  <si>
+    <t>PF18F19(24B15CS215) -AI LAB//PRM/SHIVANI/KAKUL</t>
   </si>
   <si>
     <t>LF7F8(24B11CS223) -123/PRM</t>
@@ -285,7 +275,7 @@
 LE1E2(24B41EC211) -226/ANG</t>
   </si>
   <si>
-    <t>LF5F6(24B11CS223) 148/KNS</t>
+    <t>LF5F6(24B11CS221) 148/TWT</t>
   </si>
   <si>
     <t>LE3E4(24B41EC211) -226/ANG</t>
@@ -294,7 +284,7 @@
     <t>LF3F4(24B11CS223) -111/NRP</t>
   </si>
   <si>
-    <t>LF18F19(24B15CS221) -118/SHIVANI</t>
+    <t>LF18F19(24B15CS221) -118/VARSHA</t>
   </si>
   <si>
     <t>LF13F14(24B11CS221) -153/MIT
@@ -334,6 +324,9 @@
     <t>TE3(18B11EC214) -244/MEA</t>
   </si>
   <si>
+    <t>LF16F17(24B11CS221) -111/MHS</t>
+  </si>
+  <si>
     <t>TE4(24B41EC211) -244B/ANK</t>
   </si>
   <si>
@@ -347,7 +340,10 @@
     <t>LF18F19(24B11CS222) -123/JSH</t>
   </si>
   <si>
-    <t>LALL((25B42EC211) -228/ISC</t>
+    <t>TF19(24B11CS225) -123/TWINKLE</t>
+  </si>
+  <si>
+    <t>LALL((25B42EC211) -CR53/ISC</t>
   </si>
   <si>
     <t>LF12F13F14F16F18F19E1E2E3E4
@@ -360,7 +356,7 @@
     <t>LF13F14(25B11EC311) -117/PRK</t>
   </si>
   <si>
-    <t>LF10F11F12(25B12CS211) -148/GSH</t>
+    <t>LF10F11F12(25B12CS211) -148/JSH</t>
   </si>
   <si>
     <t>LE3E4(24B41EC211) -CR54/ANG</t>
@@ -372,10 +368,10 @@
     <t>LF1F2F3(19B13BT211) -SR05/MANISHA</t>
   </si>
   <si>
-    <t>PF1F2(XXXXXXX) -CL4/KHM/MHS</t>
-  </si>
-  <si>
-    <t>LF5F6(24B11CS221) -CR53/TWT</t>
+    <t>PF1F2(XXXXXXX) -CL4/KHM/NISHANT</t>
+  </si>
+  <si>
+    <t>LF5F6(24B11CS223) -CR53/KNS</t>
   </si>
   <si>
     <t>LALL(21B12CS319) -244/RAS</t>
@@ -384,7 +380,7 @@
     <t>LF5F6(XXXXXXX) -111/MSH</t>
   </si>
   <si>
-    <t>PF7F8F9(24B15CS221) - CL2/KSA/ANU/N/SHIVANI/AVINASH/VAIBHAV</t>
+    <t>PF7F8F9(24B15CS221) - CL2/KSA/ANU/N/SHIVANI/AVINASH</t>
   </si>
   <si>
     <t>LF13F14(24B11CS223) -3037/VKG</t>
@@ -403,7 +399,7 @@
 (15B1NHS433) -229/SAV</t>
   </si>
   <si>
-    <t>PF10F11F12(24B15CS222) -151/MGO/SHR/AYP/ZUBAIR</t>
+    <t>PF10F11F12(24B15CS222) -151/MGO/SHR/AYP/FARAZ</t>
   </si>
   <si>
     <t>LF7F8(25B11EC311) -153/RUS</t>
@@ -425,7 +421,7 @@
     <t>PF16F17(24B15CS225) -AI LAB/JRD/DVG/TWINKLE</t>
   </si>
   <si>
-    <t>LF16F17(24B11CS221) -3029/MHS</t>
+    <t>LF16F17(24B11CS221) -3029/DTS</t>
   </si>
   <si>
     <t>LF7F8(24B11CS222) -153/AYP</t>
@@ -438,10 +434,10 @@
   </si>
   <si>
     <t>LF5F6(25B11EC311) -111/RUS
-TF5(24B11CS221) -225/SAMARTH</t>
-  </si>
-  <si>
-    <t>LF18F19(24B15CS221) -111/SHIVANI</t>
+TF5(24B11CS221) -225/BAIBHAV</t>
+  </si>
+  <si>
+    <t>LF18F19(24B15CS221) -111/VARSHA</t>
   </si>
   <si>
     <t>LF9F10(24B11CS222) -111/SHR</t>
@@ -450,8 +446,8 @@
     <t>LF11F12(24B11CS221)- 118/ANU</t>
   </si>
   <si>
-    <t>TF12F14F16F17F18F19E1E2E3E4
-(15B1NHS431) -234/EKS</t>
+    <t>TF14F16F17F19E1E2E4(15B1NHS431) -234
+/EKS</t>
   </si>
   <si>
     <t>PE4(15B17EC471) -142/ATK/BHC/DKS</t>
@@ -480,6 +476,9 @@
     <t>LF3F4(25B11EC311) -SR05/DIVYA</t>
   </si>
   <si>
+    <t>LF11F12(24B11CS222) -123/AMS</t>
+  </si>
+  <si>
     <t>LF9F10(25B11EC311) -111/PAA</t>
   </si>
   <si>
@@ -490,7 +489,7 @@
     <t>PF4(25B15EC311) -257/VIT/BAB/MAK</t>
   </si>
   <si>
-    <t>TF19(24B11CS221) -127/BAIBHAV</t>
+    <t>TF19(24B11CS221) -127/VARSHA</t>
   </si>
   <si>
     <t>TF12F14F16F17F18F19E1E2E3E4
@@ -503,10 +502,10 @@
     <t>TF6(24B11CS221) -229/JATIN</t>
   </si>
   <si>
+    <t>LF5F6(25B11EC311) -138//RUS</t>
+  </si>
+  <si>
     <t>THUR</t>
-  </si>
-  <si>
-    <t>LF3F4(24B11CS223) -3029/NRP</t>
   </si>
   <si>
     <t>LE3E4(24B41EC312) -111/HIG</t>
@@ -540,20 +539,23 @@
 -117/RHN</t>
   </si>
   <si>
-    <t>PF7F8F9(24B15CS222) -151/MGO/AMS/AKS</t>
+    <t>PF7F8F9(24B15CS222) -151/MGO/AMS/AKS/NISHANT</t>
   </si>
   <si>
     <t>LF1F2F3F4F5F6F7F8F9F10F11
 (25B12CS212) -117/HMV</t>
   </si>
   <si>
+    <t>LALL((25B42EC211) -228/ISC</t>
+  </si>
+  <si>
     <t>LF9F10(24B11CS221) -153/DTS</t>
   </si>
   <si>
-    <t>LF10F11F12(25B12CS211) -SR05/GSH</t>
-  </si>
-  <si>
-    <t>PF3F4(XXXXXXX) -CL4/ANK/JYR</t>
+    <t>LE1E2(24B41EC211) -244B/ANG</t>
+  </si>
+  <si>
+    <t>PF3(XXXXXXX) -CYBER SECURITY//BHB/JYR</t>
   </si>
   <si>
     <t>LF4F5F6(25B12CS211) -SR05/AKS</t>
@@ -565,19 +567,13 @@
     <t>LF11F12(24B11CS222) -3037/AMS</t>
   </si>
   <si>
-    <t>LF3F4(24B11CS221) -138/KSA</t>
-  </si>
-  <si>
     <t>PF18F19(24B15CS225) -AI LAB/DVG/TWINKLE/JRD</t>
   </si>
   <si>
     <t>LF13F14(24B11CS221) -111/MIT</t>
   </si>
   <si>
-    <t>LF3F4(25B11EC311) -117/DIVYA</t>
-  </si>
-  <si>
-    <t>LF18F19(24B15CS221) -3096/SHIVANI</t>
+    <t>LF18F19(24B15CS221) -3096/VARSHA</t>
   </si>
   <si>
     <t>LF5F6(24B11CS221) -148/TWT</t>
@@ -592,9 +588,6 @@
     <t>LF11F12(24B11CS223) -118/SHR</t>
   </si>
   <si>
-    <t>LF5F6(25B11EC311) -118//RUS</t>
-  </si>
-  <si>
     <t>LE1E2(15B11EC411) -244B/BHC</t>
   </si>
   <si>
@@ -604,7 +597,7 @@
     <t>PE4(24B45EC211) -256/DIJ/VIT</t>
   </si>
   <si>
-    <t>TF17(24B11CS221) -138/SHIVANI</t>
+    <t>TF17(24B11CS221) -138/SAMARTH</t>
   </si>
   <si>
     <t>LF1F2(25B11EC311) -111/DIVYA</t>
@@ -616,9 +609,6 @@
     <t>TF13(24B11CS221) -127/VAIBHAV</t>
   </si>
   <si>
-    <t>LE1E2(24B41EC211) -244B/ANG</t>
-  </si>
-  <si>
     <t>PF1(25B15EC311) -257/DIVYA/AJK</t>
   </si>
   <si>
@@ -658,18 +648,31 @@
     <t>TF3F4F5F6F13(15B1NHS431) -229/EKS</t>
   </si>
   <si>
+    <t>LF3F4(24B11CS223) -117/NRP</t>
+  </si>
+  <si>
+    <t>LF3F4(25B11EC311) -3029/DIVYA</t>
+  </si>
+  <si>
     <t>LF5F6(25B11EC311) -148/RUS</t>
   </si>
   <si>
     <t>TF3F4F5F6F13(16B1NHS431) -234/PRS</t>
+  </si>
+  <si>
+    <t>PF4(XXXXXXX) -APPLE LAB//BHB/JYR</t>
   </si>
   <si>
     <t>TF3F4F5F6F13(16B1NHS332)-226
 /ALOK</t>
   </si>
   <si>
-    <t>TF3F4F5F6F13((23B12HS211)-228
-/HIMANSHI</t>
+    <t>TF3F4F5F6F13((23B12HS211)-
+CR53/HIMANSHI</t>
+  </si>
+  <si>
+    <t>TF3F4F5F6F13(19B12HS412) -
+CR54/AMB</t>
   </si>
   <si>
     <t>TF3F4F5F6F13(15B1NHS433)-230/AKS</t>
@@ -678,19 +681,16 @@
     <t>FRI</t>
   </si>
   <si>
+    <t>LF3F4(25B11EC311) -153/DIVYA</t>
+  </si>
+  <si>
     <t>LF18F19(24B11CS223) -111/KHM</t>
   </si>
   <si>
     <t>LF4F5F6(19B13BT211) -117/APURVA</t>
   </si>
   <si>
-    <t>LF16F17(24B11CS221) -111/MHS</t>
-  </si>
-  <si>
-    <t>PF13F14F16(24B15CS221) - CL2/NFCS1</t>
-  </si>
-  <si>
-    <t>LF3F4(24B11CS222) -148/SGU</t>
+    <t>PF13F14F16(24B15CS221) - CL2/VAIBHAV/NAVED/KSA/TWINKLE HANDA</t>
   </si>
   <si>
     <t>PF12(25B15EC311) -257/AJK/RUS</t>
@@ -706,6 +706,9 @@
     <t>PF10F11F12F13(25B16CS211)-035/ADS/AKB</t>
   </si>
   <si>
+    <t>TF16(24B11CS225) -111/TWINKLE HANDA</t>
+  </si>
+  <si>
     <t>PF5F6(XXXXXXX) -CL4/HMA/ANK/RHN</t>
   </si>
   <si>
@@ -736,7 +739,7 @@
     <t>PE2(15B17EC471) -142/BHC/VKM</t>
   </si>
   <si>
-    <t>LF11F12(24B11CS222) -123/AMS</t>
+    <t>LF9F10(25B11EC311) -148/PAA</t>
   </si>
   <si>
     <t>LF18F19(24B11CS225) -111/JRD</t>
@@ -760,10 +763,10 @@
     <t>LE1E2(24B41EC312) -CR53/HIG</t>
   </si>
   <si>
-    <t>TF1(24B11CS221) -116/JATIN</t>
-  </si>
-  <si>
-    <t>LF3F4(25B11EC311) -153/DIVYA</t>
+    <t>TF1(24B11CS221) -126/JATIN</t>
+  </si>
+  <si>
+    <t>LF7F8(24B11CS221) -117/VARSHA</t>
   </si>
   <si>
     <t>TF7F8F3(19B12HS412)-116/AMA</t>
@@ -779,53 +782,53 @@
     <t>LF18F19(24B11CS222) -153/JSH</t>
   </si>
   <si>
-    <t>LF7F8(24B11CS221) -117/VARSHA</t>
-  </si>
-  <si>
-    <t>LF3F4(24B11CS223) -153/NRP</t>
+    <t>LF9F10(24B11CS222) -148/SHR</t>
   </si>
   <si>
     <t>TE3(15B11EC411) --121/ATK
 LF7F8(25B11EC311) -148/RUS</t>
   </si>
   <si>
-    <t>TF9(24B11CS221) -229MHS</t>
-  </si>
-  <si>
-    <t>TF3(24B11CS221) -126/VAIBHAV</t>
+    <t>TF9(24B11CS221) -229/DHRUV</t>
   </si>
   <si>
     <t>LF13F14(25B11EC311) -148/PRK</t>
   </si>
   <si>
-    <t>LF9F10(24B11CS222) -148/SHR</t>
-  </si>
-  <si>
-    <t>LF9F10(25B11EC311) -148/PAA</t>
+    <t>LF11F12(25B11EC311) -123/PAA</t>
+  </si>
+  <si>
+    <t>LF10F11F12(25B12CS211) -SR05/JSH</t>
   </si>
   <si>
     <t>TE1(18B11EC214) -244/SVS</t>
   </si>
   <si>
-    <t>TF16(24B11CS225) -127/TWINKLE</t>
-  </si>
-  <si>
-    <t>LF11F12(25B11EC311) -123/PAA</t>
+    <t>TF3(24B11CS221) -127/VAIBHAV</t>
+  </si>
+  <si>
+    <t>LF16F17F18(19B13BT211) -SR05/GUNJAN</t>
+  </si>
+  <si>
+    <t>LF3F4(24B11CS222) -SR05/SGU</t>
   </si>
   <si>
     <t>TE2(24B41EC211) -244B/ANK</t>
   </si>
   <si>
+    <t>LF3F4(24B11CS223) -3093/NRP</t>
+  </si>
+  <si>
     <t>LE3E4(18B11EC214) -111/MEA</t>
   </si>
   <si>
     <t>SAT</t>
   </si>
   <si>
-    <t>PF5(25B15EC311)-257/RUS/DIJ</t>
-  </si>
-  <si>
-    <t>PF17F18F19(24B15CS221) - CL2//NRP/S/SHIVANI/KSA/AVINASH</t>
+    <t>PF5(25B15EC311)-257/RUS/DIJ/MAK</t>
+  </si>
+  <si>
+    <t>PF17F18F19(24B15CS221) - CL2//NRP/S/SHIVANI/AVINASH/ANU</t>
   </si>
   <si>
     <t>LE1E2(18B11EC214) -111/SVS</t>
@@ -867,14 +870,13 @@
     <t>LE1E2(24B41EC312) -111/HIG</t>
   </si>
   <si>
-    <t>PF16F17(24B15CS215) -AI LAB/SHIVANI</t>
+    <t>PF16F17(24B15CS215) -AI LAB/SHIVANI/KAKUL</t>
   </si>
   <si>
     <t>LF7F8(24B11CS223) -117/PRM</t>
   </si>
   <si>
-    <t>LF18F19(24B11CS223) -CR53/KHM
-LF1F2(24B11CS221) -118/NRP</t>
+    <t>LF18F19(24B11CS223) -CR53/KHM</t>
   </si>
   <si>
     <t>LF9F10(XXXXXXX) -123/RHN</t>
@@ -895,7 +897,7 @@
     <t>TE4(15B11EC411) -116/ATK</t>
   </si>
   <si>
-    <t>TF10(24B11CS221) -229/BAIBHAV</t>
+    <t>TF10(24B11CS221) -229/VAIBHAV</t>
   </si>
   <si>
     <t>TF4(24B11CS221) -CR53/SAMARTH</t>
@@ -1496,6 +1498,10 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1702,15 +1708,15 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="58.57"/>
-    <col customWidth="1" min="2" max="2" width="55.43"/>
-    <col customWidth="1" min="3" max="3" width="63.29"/>
-    <col customWidth="1" min="4" max="4" width="58.43"/>
-    <col customWidth="1" min="5" max="5" width="79.0"/>
-    <col customWidth="1" min="6" max="6" width="79.43"/>
-    <col customWidth="1" min="7" max="7" width="99.14"/>
-    <col customWidth="1" min="8" max="8" width="82.71"/>
-    <col customWidth="1" min="9" max="9" width="71.57"/>
+    <col customWidth="1" min="1" max="1" width="43.14"/>
+    <col customWidth="1" min="2" max="2" width="51.0"/>
+    <col customWidth="1" min="3" max="3" width="43.14"/>
+    <col customWidth="1" min="4" max="4" width="104.0"/>
+    <col customWidth="1" min="5" max="5" width="65.14"/>
+    <col customWidth="1" min="6" max="6" width="45.14"/>
+    <col customWidth="1" min="7" max="7" width="60.43"/>
+    <col customWidth="1" min="8" max="8" width="52.0"/>
+    <col customWidth="1" min="9" max="9" width="98.57"/>
     <col customWidth="1" min="10" max="26" width="8.71"/>
   </cols>
   <sheetData>
@@ -1822,12 +1828,6 @@
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1840,25 +1840,22 @@
       <c r="H8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="9">
       <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>40</v>
@@ -1868,14 +1865,20 @@
       <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>44</v>
+        <v>19</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11">
@@ -1885,380 +1888,383 @@
       <c r="C11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="B21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="B22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="B23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="C24" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="C25" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="C26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="C27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="D27" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="D30" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="B31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="B33" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="B34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="B35" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="B36" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="B37" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="B38" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>147</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -2287,16 +2293,17 @@
         <v>154</v>
       </c>
     </row>
-    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="D42" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="B44" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="C44" s="1" t="s">
         <v>157</v>
       </c>
@@ -2341,38 +2348,38 @@
         <v>168</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>106</v>
+        <v>169</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="B47" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="B48" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>175</v>
+        <v>76</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>176</v>
@@ -2381,112 +2388,112 @@
         <v>177</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>178</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="B49" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="B50" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="B51" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="B52" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="B53" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E53" s="1" t="s">
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="B54" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="D54" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="H54" s="1" t="s">
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="D55" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
       <c r="H55" s="1" t="s">
         <v>208</v>
       </c>
@@ -2502,321 +2509,321 @@
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="1" t="s">
+      <c r="H58" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="I58" s="1" t="s">
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="A59" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="B59" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="I59" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="B60" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="B61" s="1" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="B62" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H62" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="B63" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I63" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="B64" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I64" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="B65" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="B66" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H66" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="B67" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="68" ht="15.75" customHeight="1">
+      <c r="C68" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="E68" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="G68" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="G67" s="1" t="s">
+      <c r="H68" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
-      <c r="B68" s="1" t="s">
+    <row r="69" ht="15.75" customHeight="1">
+      <c r="B69" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G68" s="1" t="s">
+      <c r="G69" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="69" ht="15.75" customHeight="1"/>
     <row r="70" ht="15.75" customHeight="1">
+      <c r="B70" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="D70" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
+    <row r="72" ht="15.75" customHeight="1"/>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="B73" s="1" t="s">
+      <c r="A73" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="B74" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="B75" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="B76" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="B77" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="B78" s="1" t="s">
-        <v>226</v>
+        <v>269</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="B79" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="B80" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D80" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="E80" s="1" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1">
+      <c r="B83" s="1" t="s">
+        <v>277</v>
+      </c>
       <c r="C83" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D83" s="1" t="s">
+    </row>
+    <row r="84" ht="15.75" customHeight="1">
+      <c r="C84" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="84" ht="15.75" customHeight="1">
-      <c r="B84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D84" s="1" t="s">
+    </row>
+    <row r="85" ht="15.75" customHeight="1">
+      <c r="B85" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="85" ht="15.75" customHeight="1">
-      <c r="D85" s="1" t="s">
+      <c r="E85" s="1" t="s">
         <v>284</v>
       </c>
     </row>
@@ -2825,646 +2832,634 @@
         <v>285</v>
       </c>
     </row>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1">
-      <c r="B88" s="1" t="s">
+    <row r="87" ht="15.75" customHeight="1">
+      <c r="D87" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="I88" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
+    </row>
+    <row r="88" ht="15.75" customHeight="1"/>
     <row r="89" ht="15.75" customHeight="1">
       <c r="B89" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="G89" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D89" s="1" t="s">
+      <c r="H89" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I89" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="I89" s="1" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="B90" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="I90" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="B91" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="I91" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="B92" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I92" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="H92" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="B93" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="I93" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="I93" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="B94" s="1" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="D94" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="I94" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="H94" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="I94" s="1" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="B95" s="1" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="I95" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="B96" s="1" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="F96" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I96" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="H96" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="B97" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="I97" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="H97" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="B98" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="I98" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="B99" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="I99" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="H99" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="B100" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="I100" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="H100" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="B101" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="I101" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="H101" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="B102" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="I102" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="H102" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="I102" s="1" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="B103" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="I103" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="H103" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="I103" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="B104" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="I104" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="B105" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E105" s="1" t="s">
         <v>399</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="B106" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>402</v>
-      </c>
       <c r="D106" s="1" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="B107" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E107" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="B108" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E108" s="1" t="s">
         <v>409</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="B109" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="E109" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="B110" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>291</v>
+        <v>414</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="B111" s="1" t="s">
-        <v>316</v>
+        <v>291</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>317</v>
+        <v>292</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="B112" s="1" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="B113" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="B114" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E114" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="B115" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="E115" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="B116" s="1" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="D116" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>427</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="B117" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E117" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="B118" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="E118" s="1" t="s">
         <v>431</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="B119" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="E119" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1"/>
     <row r="121" ht="15.75" customHeight="1"/>
     <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
@@ -3472,150 +3467,166 @@
         <v>438</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>439</v>
+        <v>422</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>440</v>
+        <v>287</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>441</v>
+        <v>288</v>
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F124" s="1" t="s">
         <v>442</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="F125" s="1" t="s">
         <v>446</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="1" t="s">
-        <v>432</v>
+        <v>447</v>
       </c>
       <c r="B126" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="F126" s="1" t="s">
         <v>451</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="1" t="s">
-        <v>341</v>
+        <v>433</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>420</v>
+        <v>452</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>442</v>
+        <v>453</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="E127" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="F127" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="1" t="s">
-        <v>417</v>
+        <v>342</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="C128" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="F128" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="1" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="E129" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="F129" s="1" t="s">
         <v>460</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="1" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="B130" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="131" ht="15.75" customHeight="1">
+      <c r="A131" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="C130" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="F130" s="1" t="s">
+      <c r="B131" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="E131" s="1" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="131" ht="15.75" customHeight="1"/>
+      <c r="F131" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
     <row r="132" ht="15.75" customHeight="1"/>
     <row r="133" ht="15.75" customHeight="1"/>
     <row r="134" ht="15.75" customHeight="1"/>
@@ -4486,7 +4497,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="84">
+  <mergeCells count="85">
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="B5:C5"/>
@@ -4510,39 +4521,39 @@
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="D46:E46"/>
     <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:F49"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="F34:F38"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="F46:F57"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:F58"/>
+    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="F64:F72"/>
+    <mergeCell ref="C65:D65"/>
     <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="F72:F80"/>
-    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="A59:A72"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="F83:F87"/>
+    <mergeCell ref="A88:A103"/>
+    <mergeCell ref="A104:A119"/>
+    <mergeCell ref="A73:A87"/>
+    <mergeCell ref="F73:F80"/>
+    <mergeCell ref="B74:C74"/>
     <mergeCell ref="D74:E74"/>
     <mergeCell ref="D75:E75"/>
     <mergeCell ref="D76:E76"/>
     <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="F63:F71"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="G66:H66"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="B6:C6"/>
@@ -4556,21 +4567,22 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="C22:E22"/>
+    <mergeCell ref="A16:A28"/>
+    <mergeCell ref="A43:A58"/>
+    <mergeCell ref="A29:A42"/>
     <mergeCell ref="H44:I44"/>
     <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H87:I87"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="F83:F86"/>
-    <mergeCell ref="A87:A102"/>
-    <mergeCell ref="A103:A119"/>
-    <mergeCell ref="A16:A28"/>
-    <mergeCell ref="A43:A57"/>
-    <mergeCell ref="A58:A71"/>
-    <mergeCell ref="A29:A42"/>
-    <mergeCell ref="A72:A86"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="F34:F38"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="D45:E45"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>

</xml_diff>

<commit_message>
chore: update 128 btech sem4, btech62 sem2,4
</commit_message>
<xml_diff>
--- a/raw/time_tables/B.Tech 128 (btech-128)/4/1.xlsx
+++ b/raw/time_tables/B.Tech 128 (btech-128)/4/1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="466">
   <si>
     <t>B.TECH. II Yr( IV SEMESTER) TIMETABLE EVEN SEMESTER 2026, JIIT-128</t>
   </si>
@@ -37,8 +37,11 @@
     <t>2:00 PM - 2:50 PM</t>
   </si>
   <si>
-    <t>3:00 PM - 3 :50 PM
-4:00 PM -4:50 PM</t>
+    <t xml:space="preserve">3:00 PM - 3 :50 PM
+</t>
+  </si>
+  <si>
+    <t>4:00 PM -4:50 PM</t>
   </si>
   <si>
     <t>MON</t>
@@ -1483,11 +1486,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1747,1884 +1753,1887 @@
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="H17" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="B22" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="C24" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="C25" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="C26" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="C27" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="D30" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="B31" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="B33" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="B34" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="B35" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="B36" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="B37" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="B38" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1">
       <c r="D41" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="D42" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="C44" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="B45" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="B46" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="B47" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="B48" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="B49" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="B50" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="B51" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="B52" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="B53" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="B54" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="D55" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="H56" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="H57" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="H58" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="B60" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D60" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="G60" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="H60" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="B61" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="B62" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="B63" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="B64" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="B65" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="B66" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="B67" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="C68" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="B69" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="B70" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1"/>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="B74" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="B75" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="B76" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="B77" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="B78" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="B79" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="B80" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1">
       <c r="B83" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="C84" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="B85" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="D86" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="D87" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1"/>
     <row r="89" ht="15.75" customHeight="1">
       <c r="B89" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C89" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>287</v>
-      </c>
       <c r="E89" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G89" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H89" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="H89" s="1" t="s">
-        <v>289</v>
-      </c>
       <c r="I89" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="B90" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>291</v>
-      </c>
       <c r="E90" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="B91" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="E91" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="B92" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="E92" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="B93" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="B94" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="B95" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="B96" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="B97" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="B98" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="B99" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="B100" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="B101" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="B102" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="B103" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="B104" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="B105" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="B106" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="B107" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="B108" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="B109" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="B110" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="B111" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="B112" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="B113" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="B114" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="B115" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="B116" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="B117" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="B118" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="B119" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1"/>
     <row r="121" ht="15.75" customHeight="1"/>
     <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="132" ht="15.75" customHeight="1"/>
@@ -4497,7 +4506,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="85">
+  <mergeCells count="84">
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="B5:C5"/>
@@ -4532,34 +4541,33 @@
     <mergeCell ref="F60:F62"/>
     <mergeCell ref="D62:E62"/>
     <mergeCell ref="D63:E63"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
     <mergeCell ref="C64:D64"/>
     <mergeCell ref="F64:F72"/>
     <mergeCell ref="C65:D65"/>
+    <mergeCell ref="F73:F80"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F83:F87"/>
+    <mergeCell ref="A73:A87"/>
+    <mergeCell ref="A88:A103"/>
+    <mergeCell ref="A104:A119"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="A59:A72"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="D60:E60"/>
-    <mergeCell ref="B61:C61"/>
     <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D78:E78"/>
     <mergeCell ref="B80:C80"/>
-    <mergeCell ref="F83:F87"/>
-    <mergeCell ref="A88:A103"/>
-    <mergeCell ref="A104:A119"/>
-    <mergeCell ref="A73:A87"/>
-    <mergeCell ref="F73:F80"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="H2:I2"/>
     <mergeCell ref="A3:A15"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B4:C4"/>
@@ -4568,8 +4576,8 @@
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="A16:A28"/>
+    <mergeCell ref="A29:A42"/>
     <mergeCell ref="A43:A58"/>
-    <mergeCell ref="A29:A42"/>
     <mergeCell ref="H44:I44"/>
     <mergeCell ref="H45:I45"/>
     <mergeCell ref="H61:I61"/>

</xml_diff>